<commit_message>
Modification des données des entreprise + création des données des stage
</commit_message>
<xml_diff>
--- a/Sprint 1/Global/BD/employeEntreprise.xlsx
+++ b/Sprint 1/Global/BD/employeEntreprise.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poifr1532452\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\poifr1532452\Desktop\Projet\Sprint 1\Global\BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,7 +1284,7 @@
         <v>45210</v>
       </c>
       <c r="H2" s="2">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1310,7 +1310,7 @@
         <v>84300</v>
       </c>
       <c r="H3" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1336,7 +1336,7 @@
         <v>38486</v>
       </c>
       <c r="H4" s="2">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>11568</v>
       </c>
       <c r="H5" s="2">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1388,7 +1388,7 @@
         <v>81068</v>
       </c>
       <c r="H6" s="2">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1414,7 +1414,7 @@
         <v>1590</v>
       </c>
       <c r="H7" s="2">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1440,7 +1440,7 @@
         <v>7660</v>
       </c>
       <c r="H8" s="2">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1466,7 +1466,7 @@
         <v>95090</v>
       </c>
       <c r="H9" s="2">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -1492,7 +1492,7 @@
         <v>48771</v>
       </c>
       <c r="H10" s="2">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1518,7 +1518,7 @@
         <v>61301</v>
       </c>
       <c r="H11" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1544,7 +1544,7 @@
         <v>55978</v>
       </c>
       <c r="H12" s="2">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1570,7 +1570,7 @@
         <v>22240</v>
       </c>
       <c r="H13" s="2">
-        <v>39</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1596,7 +1596,7 @@
         <v>62318</v>
       </c>
       <c r="H14" s="2">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1648,7 +1648,7 @@
         <v>40000</v>
       </c>
       <c r="H16" s="2">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1674,7 +1674,7 @@
         <v>9048</v>
       </c>
       <c r="H17" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1700,7 +1700,7 @@
         <v>25150</v>
       </c>
       <c r="H18" s="2">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1726,7 +1726,7 @@
         <v>35635</v>
       </c>
       <c r="H19" s="2">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1752,7 +1752,7 @@
         <v>23807</v>
       </c>
       <c r="H20" s="2">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
         <v>88543</v>
       </c>
       <c r="H21" s="2">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1804,7 +1804,7 @@
         <v>96764</v>
       </c>
       <c r="H22" s="2">
-        <v>34</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1830,7 +1830,7 @@
         <v>76172</v>
       </c>
       <c r="H23" s="2">
-        <v>49</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1856,7 +1856,7 @@
         <v>44529</v>
       </c>
       <c r="H24" s="2">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1882,7 +1882,7 @@
         <v>92974</v>
       </c>
       <c r="H25" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1908,7 +1908,7 @@
         <v>71332</v>
       </c>
       <c r="H26" s="2">
-        <v>46</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1934,7 +1934,7 @@
         <v>89589</v>
       </c>
       <c r="H27" s="2">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -1960,7 +1960,7 @@
         <v>44330</v>
       </c>
       <c r="H28" s="2">
-        <v>44</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -1986,7 +1986,7 @@
         <v>75416</v>
       </c>
       <c r="H29" s="2">
-        <v>29</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2012,7 +2012,7 @@
         <v>92105</v>
       </c>
       <c r="H30" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2038,7 +2038,7 @@
         <v>63195</v>
       </c>
       <c r="H31" s="2">
-        <v>39</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2064,7 +2064,7 @@
         <v>37939</v>
       </c>
       <c r="H32" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2090,7 +2090,7 @@
         <v>23838</v>
       </c>
       <c r="H33" s="2">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2116,7 +2116,7 @@
         <v>33322</v>
       </c>
       <c r="H34" s="2">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2142,7 +2142,7 @@
         <v>67301</v>
       </c>
       <c r="H35" s="2">
-        <v>34</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2168,7 +2168,7 @@
         <v>11835</v>
       </c>
       <c r="H36" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
         <v>94802</v>
       </c>
       <c r="H37" s="2">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2220,7 +2220,7 @@
         <v>82768</v>
       </c>
       <c r="H38" s="2">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2246,7 +2246,7 @@
         <v>55421</v>
       </c>
       <c r="H39" s="2">
-        <v>48</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2272,7 +2272,7 @@
         <v>48284</v>
       </c>
       <c r="H40" s="2">
-        <v>25</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
@@ -2298,7 +2298,7 @@
         <v>3022</v>
       </c>
       <c r="H41" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -2324,7 +2324,7 @@
         <v>85190</v>
       </c>
       <c r="H42" s="2">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
@@ -2350,7 +2350,7 @@
         <v>11335</v>
       </c>
       <c r="H43" s="2">
-        <v>41</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -2376,7 +2376,7 @@
         <v>82475</v>
       </c>
       <c r="H44" s="2">
-        <v>44</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -2402,7 +2402,7 @@
         <v>68763</v>
       </c>
       <c r="H45" s="2">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -2428,7 +2428,7 @@
         <v>64494</v>
       </c>
       <c r="H46" s="2">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
         <v>93011</v>
       </c>
       <c r="H47" s="2">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -2506,7 +2506,7 @@
         <v>48661</v>
       </c>
       <c r="H49" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2532,7 +2532,7 @@
         <v>93761</v>
       </c>
       <c r="H50" s="2">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>